<commit_message>
change to current PL rank
</commit_message>
<xml_diff>
--- a/output/c6/c6aurac_brawler_levels_team.xlsx
+++ b/output/c6/c6aurac_brawler_levels_team.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>player</t>
   </si>
@@ -28,10 +28,10 @@
     <t>trophies</t>
   </si>
   <si>
-    <t>highest_pl_rank_score</t>
-  </si>
-  <si>
-    <t>highest_pl_rank</t>
+    <t>pl_score</t>
+  </si>
+  <si>
+    <t>pl_rank</t>
   </si>
   <si>
     <t>level_9s</t>
@@ -220,33 +220,27 @@
     <t>#GJCYYV0P</t>
   </si>
   <si>
+    <t>Silver III</t>
+  </si>
+  <si>
+    <t>Diamond III</t>
+  </si>
+  <si>
+    <t>Diamond II</t>
+  </si>
+  <si>
+    <t>Mythic II</t>
+  </si>
+  <si>
+    <t>Gold II</t>
+  </si>
+  <si>
     <t>Diamond I</t>
   </si>
   <si>
-    <t>Gold II</t>
-  </si>
-  <si>
-    <t>Gold III</t>
-  </si>
-  <si>
-    <t>Diamond II</t>
-  </si>
-  <si>
-    <t>Diamond III</t>
-  </si>
-  <si>
-    <t>Mythic III</t>
-  </si>
-  <si>
     <t>Gold I</t>
   </si>
   <si>
-    <t>Mythic I</t>
-  </si>
-  <si>
-    <t>Mythic II</t>
-  </si>
-  <si>
     <t>Legend I</t>
   </si>
   <si>
@@ -316,7 +310,7 @@
     <t xml:space="preserve">BARLEY, BELLE, BIBI, BO, BYRON, COLT, CROW, DARRYL, EMZ, EVE, GRIFF, LOU, ... </t>
   </si>
   <si>
-    <t xml:space="preserve">ASH, BELLE, BO, BROCK, CARL, COLETTE, CROW, DARRYL, EDGAR, EMZ, GALE, GRIFF, ... </t>
+    <t xml:space="preserve">ASH, BEA, BELLE, BO, BROCK, CARL, COLETTE, CROW, DARRYL, EDGAR, EMZ, GALE, ... </t>
   </si>
   <si>
     <t>MORTIS, RICO</t>
@@ -721,7 +715,7 @@
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -770,7 +764,7 @@
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -782,22 +776,20 @@
         <v>35077</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2">
         <v>31</v>
       </c>
       <c r="H2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2" s="2">
         <v>27</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -846,22 +838,20 @@
         <v>35077</v>
       </c>
       <c r="E4" s="2">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2">
         <v>31</v>
       </c>
       <c r="H4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="2">
         <v>27</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -875,13 +865,13 @@
         <v>40</v>
       </c>
       <c r="D5" s="2">
-        <v>29721</v>
+        <v>29764</v>
       </c>
       <c r="E5" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="2">
         <v>40</v>
@@ -893,7 +883,7 @@
         <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -910,13 +900,11 @@
         <v>35728</v>
       </c>
       <c r="E6" s="2">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="2">
         <v>8</v>
@@ -925,7 +913,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -942,11 +930,9 @@
         <v>23950</v>
       </c>
       <c r="E7" s="2">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2">
         <v>21</v>
       </c>
@@ -954,10 +940,10 @@
         <v>3</v>
       </c>
       <c r="I7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -977,7 +963,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G8" s="2">
         <v>27</v>
@@ -989,7 +975,7 @@
         <v>13</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -1009,7 +995,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9" s="2">
         <v>28</v>
@@ -1021,7 +1007,7 @@
         <v>11</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -1038,10 +1024,10 @@
         <v>36451</v>
       </c>
       <c r="E10" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G10" s="2">
         <v>23</v>
@@ -1053,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -1073,7 +1059,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1085,7 +1071,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -1105,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2">
         <v>40</v>
@@ -1117,7 +1103,7 @@
         <v>5</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -1134,13 +1120,13 @@
         <v>12401</v>
       </c>
       <c r="E13" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13" s="2">
         <v>33</v>
@@ -1149,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -1166,22 +1152,22 @@
         <v>33949</v>
       </c>
       <c r="E14" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G14" s="2">
         <v>31</v>
       </c>
       <c r="H14" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I14" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -1213,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -1230,10 +1216,10 @@
         <v>34596</v>
       </c>
       <c r="E16" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -1242,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1262,10 +1248,10 @@
         <v>33365</v>
       </c>
       <c r="E17" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G17" s="2">
         <v>11</v>
@@ -1274,10 +1260,10 @@
         <v>37</v>
       </c>
       <c r="I17" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1294,10 +1280,10 @@
         <v>16174</v>
       </c>
       <c r="E18" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G18" s="2">
         <v>10</v>
@@ -1306,10 +1292,10 @@
         <v>3</v>
       </c>
       <c r="I18" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1326,22 +1312,22 @@
         <v>31856</v>
       </c>
       <c r="E19" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G19" s="2">
         <v>33</v>
       </c>
       <c r="H19" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1358,10 +1344,10 @@
         <v>33527</v>
       </c>
       <c r="E20" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G20" s="2">
         <v>19</v>
@@ -1370,10 +1356,10 @@
         <v>22</v>
       </c>
       <c r="I20" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1390,10 +1376,10 @@
         <v>31355</v>
       </c>
       <c r="E21" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G21" s="2">
         <v>28</v>
@@ -1402,10 +1388,10 @@
         <v>16</v>
       </c>
       <c r="I21" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1422,10 +1408,10 @@
         <v>34890</v>
       </c>
       <c r="E22" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G22" s="2">
         <v>23</v>
@@ -1434,10 +1420,10 @@
         <v>12</v>
       </c>
       <c r="I22" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1454,10 +1440,10 @@
         <v>31327</v>
       </c>
       <c r="E23" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G23" s="2">
         <v>27</v>
@@ -1469,7 +1455,7 @@
         <v>9</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1489,7 +1475,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G24" s="2">
         <v>6</v>
@@ -1501,7 +1487,7 @@
         <v>14</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1518,22 +1504,22 @@
         <v>37857</v>
       </c>
       <c r="E25" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G25" s="2">
         <v>1</v>
       </c>
       <c r="H25" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="2">
         <v>21</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1547,13 +1533,13 @@
         <v>61</v>
       </c>
       <c r="D26" s="2">
-        <v>38062</v>
+        <v>38082</v>
       </c>
       <c r="E26" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G26" s="2">
         <v>17</v>
@@ -1562,10 +1548,10 @@
         <v>10</v>
       </c>
       <c r="I26" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1582,10 +1568,10 @@
         <v>8241</v>
       </c>
       <c r="E27" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G27" s="2">
         <v>24</v>
@@ -1594,10 +1580,10 @@
         <v>3</v>
       </c>
       <c r="I27" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1629,7 +1615,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1646,11 +1632,9 @@
         <v>24874</v>
       </c>
       <c r="E29" s="2">
-        <v>8</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F29" s="2"/>
       <c r="G29" s="2">
         <v>1</v>
       </c>
@@ -1661,7 +1645,7 @@
         <v>4</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1678,10 +1662,10 @@
         <v>5474</v>
       </c>
       <c r="E30" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
@@ -1693,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1710,10 +1694,10 @@
         <v>31651</v>
       </c>
       <c r="E31" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
@@ -1722,10 +1706,10 @@
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1742,11 +1726,9 @@
         <v>31160</v>
       </c>
       <c r="E32" s="2">
-        <v>12</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F32" s="2"/>
       <c r="G32" s="2">
         <v>33</v>
       </c>
@@ -1757,7 +1739,7 @@
         <v>7</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update highest pl rank
</commit_message>
<xml_diff>
--- a/output/c6/c6aurac_brawler_levels_team.xlsx
+++ b/output/c6/c6aurac_brawler_levels_team.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
   <si>
     <t>player</t>
   </si>
@@ -79,51 +79,54 @@
     <t>_mym_</t>
   </si>
   <si>
+    <t>nik haikal</t>
+  </si>
+  <si>
+    <t>axnsan</t>
+  </si>
+  <si>
+    <t>lolzorsish</t>
+  </si>
+  <si>
+    <t>xardas</t>
+  </si>
+  <si>
+    <t>LA | FLASH</t>
+  </si>
+  <si>
+    <t>Saurav</t>
+  </si>
+  <si>
+    <t>Snoopy&gt;.&lt;|をゆひせぬ</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>DOOM</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>Tribe | LHC 2</t>
+  </si>
+  <si>
+    <t>joshua</t>
+  </si>
+  <si>
+    <t>☬ℝ𝔸𝕋𝕋𝕃𝔼ℝ☬</t>
+  </si>
+  <si>
     <t>IX|LIT</t>
   </si>
   <si>
-    <t>Omz</t>
-  </si>
-  <si>
-    <t>Snoopy&gt;.&lt;|をゆひせぬ</t>
-  </si>
-  <si>
-    <t>H¥DRA|HANZLA ¢</t>
-  </si>
-  <si>
-    <t>Ninja❦</t>
-  </si>
-  <si>
-    <t>Saurav</t>
-  </si>
-  <si>
-    <t>Blaze</t>
-  </si>
-  <si>
-    <t>DOOM</t>
-  </si>
-  <si>
-    <t>eric</t>
-  </si>
-  <si>
-    <t>Tribe | LHC 2</t>
-  </si>
-  <si>
-    <t>joshua</t>
-  </si>
-  <si>
-    <t>你牛什么牛</t>
-  </si>
-  <si>
     <t>Mini Breeze</t>
   </si>
   <si>
     <t>Mini|Benn🎯</t>
   </si>
   <si>
-    <t>sasameseed</t>
-  </si>
-  <si>
     <t>RICOFTW</t>
   </si>
   <si>
@@ -166,51 +169,54 @@
     <t>#82808UG9G</t>
   </si>
   <si>
+    <t>#P00C0RR8</t>
+  </si>
+  <si>
+    <t>#2VY2PC0PL</t>
+  </si>
+  <si>
+    <t>#289GU8LR8</t>
+  </si>
+  <si>
+    <t>#2P88VGRL0</t>
+  </si>
+  <si>
+    <t>#2YCQJ00Y</t>
+  </si>
+  <si>
+    <t>#U2Q9L2QU</t>
+  </si>
+  <si>
+    <t>#C9RCCU8J</t>
+  </si>
+  <si>
+    <t>#C0R8YQC</t>
+  </si>
+  <si>
+    <t>#CPJC0QUV</t>
+  </si>
+  <si>
+    <t>#80VR8V9</t>
+  </si>
+  <si>
+    <t>#V8VRPRYQ</t>
+  </si>
+  <si>
+    <t>#C29RQJLU</t>
+  </si>
+  <si>
+    <t>#89GV9UG9Q</t>
+  </si>
+  <si>
     <t>#8V09Y2Y8</t>
   </si>
   <si>
-    <t>#8L00JQGP9</t>
-  </si>
-  <si>
-    <t>#C9RCCU8J</t>
-  </si>
-  <si>
-    <t>#8YGQJCUVR</t>
-  </si>
-  <si>
-    <t>#9JVYLJY</t>
-  </si>
-  <si>
-    <t>#U2Q9L2QU</t>
-  </si>
-  <si>
-    <t>#C0R8YQC</t>
-  </si>
-  <si>
-    <t>#CPJC0QUV</t>
-  </si>
-  <si>
-    <t>#80VR8V9</t>
-  </si>
-  <si>
-    <t>#V8VRPRYQ</t>
-  </si>
-  <si>
-    <t>#C29RQJLU</t>
-  </si>
-  <si>
-    <t>#89GV9UG9Q</t>
-  </si>
-  <si>
     <t>#2CVYPV0YP</t>
   </si>
   <si>
     <t>#9RVV02QQ</t>
   </si>
   <si>
-    <t>#8999QQCPC</t>
-  </si>
-  <si>
     <t>#9ULG0RR8V</t>
   </si>
   <si>
@@ -220,49 +226,52 @@
     <t>#GJCYYV0P</t>
   </si>
   <si>
+    <t>Diamond I</t>
+  </si>
+  <si>
+    <t>Silver III</t>
+  </si>
+  <si>
+    <t>Mythic I</t>
+  </si>
+  <si>
+    <t>Diamond III</t>
+  </si>
+  <si>
+    <t>Diamond II</t>
+  </si>
+  <si>
+    <t>Gold II</t>
+  </si>
+  <si>
+    <t>Gold I</t>
+  </si>
+  <si>
     <t>Gold III</t>
   </si>
   <si>
-    <t>Silver III</t>
-  </si>
-  <si>
-    <t>Diamond III</t>
-  </si>
-  <si>
-    <t>Diamond II</t>
-  </si>
-  <si>
     <t>Mythic II</t>
   </si>
   <si>
-    <t>Gold II</t>
-  </si>
-  <si>
-    <t>Diamond I</t>
-  </si>
-  <si>
-    <t>Gold I</t>
-  </si>
-  <si>
     <t>Legend I</t>
   </si>
   <si>
-    <t xml:space="preserve">BEA, BELLE, BIBI, BO, BROCK, BYRON, CARL, COLT, CROW, DARRYL, EMZ, EVE, ... </t>
-  </si>
-  <si>
-    <t>BARLEY, BO, CROW, DARRYL, EMZ, JESSIE, NANI, NITA, PENNY, SANDY, STU, TICK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMBER, ASH, BELLE, BONNIE, CARL, COLETTE, CROW, EVE, GALE, GENE, GRIFF, GROM, ... </t>
-  </si>
-  <si>
-    <t>DARRYL, EL PRIMO, GALE, LEON, SANDY, SPIKE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BONNIE, BROCK, BUZZ, DARRYL, EMZ, GENE, GRIFF, LOLA, MAX, MEG, PAM, POCO, ... </t>
-  </si>
-  <si>
-    <t>ASH, BEA, BUSTER, CARL, CROW, FANG, MORTIS, SPIKE, STU, SURGE</t>
+    <t xml:space="preserve">BEA, BELLE, BIBI, BO, BROCK, BUSTER, BUZZ, BYRON, CARL, CHESTER, COLT, CROW, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARLEY, BO, CROW, DARRYL, EMZ, EVE, JESSIE, NANI, NITA, PENNY, POCO, SANDY, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMBER, ASH, BEA, BELLE, BONNIE, BULL, BUSTER, CARL, CHESTER, COLETTE, CROW, EVE, ... </t>
+  </si>
+  <si>
+    <t>DARRYL, EL PRIMO, GALE, JESSIE, LEON, SANDY, SPIKE, SURGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASH, BELLE, BO, BONNIE, BROCK, BUSTER, BUZZ, CARL, COLETTE, CROW, DARRYL, EMZ, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASH, BEA, BELLE, BROCK, BUSTER, CARL, CHESTER, COLETTE, CROW, FANG, MORTIS, SPIKE, ... </t>
   </si>
   <si>
     <t>8-BIT, ASH, BIBI, TICK</t>
@@ -271,70 +280,76 @@
     <t xml:space="preserve">AMBER, ASH, BARLEY, BO, BONNIE, BROCK, BULL, BUSTER, BUZZ, BYRON, CARL, CROW, ... </t>
   </si>
   <si>
-    <t>EMZ, MORTIS, PIPER, POCO, SQUEAK</t>
+    <t>BEA, BO, EMZ, GUS, JACKY, MORTIS, PENNY, PIPER, POCO, SQUEAK</t>
   </si>
   <si>
     <t>BUZZ, PENNY</t>
   </si>
   <si>
-    <t xml:space="preserve">BEA, BO, BYRON, CARL, CROW, GENE, GRIFF, MAX, PAM, POCO, ROSA, RUFFS, ... </t>
-  </si>
-  <si>
-    <t>BIBI, MORTIS, RICO</t>
+    <t xml:space="preserve">BEA, BO, BUSTER, BYRON, CARL, CHESTER, CROW, GENE, GRIFF, MAX, PAM, POCO, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-BIT, BEA, BELLE, BO, BONNIE, BROCK, BUSTER, BUZZ, CARL, CHESTER, COLT, CROW, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-BIT, AMBER, ASH, BELLE, BO, BONNIE, BROCK, BYRON, CHESTER, COLETTE, CROW, EDGAR, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BO, BROCK, CARL, COLT, DARRYL, FRANK, GALE, GENE, LEON, NITA, PAM, POCO, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEA, BELLE, BO, BONNIE, BROCK, BUSTER, BUZZ, CARL, CHESTER, COLETTE, CROW, DARRYL, ... </t>
+  </si>
+  <si>
+    <t>COLETTE, COLT, CROW, FANG, MAX, MORTIS, STU, SURGE, TARA</t>
+  </si>
+  <si>
+    <t>BEA, CARL, COLT, EMZ, GENE, JACKY, MAX, MORTIS, SURGE, TARA</t>
+  </si>
+  <si>
+    <t>8-BIT, BUSTER, CHESTER, DYNAMIKE, EDGAR, EMZ, GRAY, MEG, PENNY, POCO, STU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BELLE, BUSTER, BYRON, CHESTER, CROW, GRIFF, GUS, JANET, OTIS, PIPER, POCO, SQUEAK, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASH, BEA, BELLE, BO, BONNIE, BUSTER, CARL, CHESTER, CROW, EMZ, EVE, GENE, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASH, BELLE, EVE, GENE, GRIFF, LOLA, LOU, NANI, POCO, SPIKE, SPROUT, SURGE, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-BIT, BONNIE, BROCK, CARL, CROW, DARRYL, EL PRIMO, EMZ, EVE, FANG, GROM, GUS, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARLEY, BELLE, BIBI, BO, BYRON, COLT, CROW, DARRYL, EMZ, EVE, GRIFF, LOU, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMBER, ASH, BEA, BELLE, BIBI, BO, BROCK, BUZZ, CARL, CHESTER, COLETTE, CROW, ... </t>
+  </si>
+  <si>
+    <t>BIBI, CHESTER, MORTIS, RICO, TARA</t>
+  </si>
+  <si>
+    <t>MORTIS, RICO</t>
+  </si>
+  <si>
+    <t>BO, DARRYL, LOLA, PAM, PENNY, RICO, SPIKE</t>
+  </si>
+  <si>
+    <t>BEA, COLT, GROM, JESSIE, PENNY, RICO, SHELLY</t>
   </si>
   <si>
     <t xml:space="preserve">8-BIT, AMBER, ASH, BARLEY, BEA, BELLE, BIBI, BO, BONNIE, BROCK, BULL, BUSTER, ... </t>
   </si>
   <si>
-    <t>8-BIT, BUSTER, EDGAR, MEG, PENNY, POCO, STU</t>
-  </si>
-  <si>
-    <t>BO, BROCK, EMZ, EVE, MAX, POCO, RICO, SANDY, SPIKE, STU</t>
-  </si>
-  <si>
-    <t>COLT, MORTIS, STU</t>
-  </si>
-  <si>
-    <t>BEA, CARL, COLT, EMZ, GENE, JACKY, MAX, MORTIS, SURGE, TARA</t>
-  </si>
-  <si>
-    <t>BELLE, BYRON, CROW, GRIFF, GUS, JANET, PIPER, POCO, SQUEAK, STU, SURGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASH, BELLE, BO, BONNIE, CARL, CROW, EMZ, EVE, GENE, GRIFF, GUS, JANET, ... </t>
-  </si>
-  <si>
-    <t>ASH, EVE, GRIFF, LOLA, LOU, NANI, POCO, SPIKE, TICK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BONNIE, BROCK, CARL, CROW, EMZ, FANG, GUS, JANET, LEON, OTIS, PENNY, POCO, ... </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BARLEY, BELLE, BIBI, BO, BYRON, COLT, CROW, DARRYL, EMZ, EVE, GRIFF, LOU, ... </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASH, BEA, BELLE, BO, BROCK, CARL, COLETTE, CROW, DARRYL, EDGAR, EMZ, GALE, ... </t>
-  </si>
-  <si>
-    <t>MORTIS, RICO</t>
-  </si>
-  <si>
-    <t>BO, DARRYL, LOLA, PAM, PENNY, RICO</t>
-  </si>
-  <si>
-    <t>CROW, EVE, MORTIS, SPIKE</t>
-  </si>
-  <si>
-    <t>COLT, GROM, JESSIE, PENNY, RICO</t>
-  </si>
-  <si>
-    <t>ASH, BYRON, EMZ, EVE, GENE, GRIFF, SANDY</t>
+    <t>ASH, BYRON, CARL, EMZ, EVE, GENE, GRIFF, SANDY, SPIKE, SURGE</t>
   </si>
   <si>
     <t>C6 Brawler Levels</t>
   </si>
   <si>
-    <t>2022-11-25</t>
+    <t>2022-12-29</t>
   </si>
 </sst>
 </file>
@@ -705,7 +720,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS32"/>
+  <dimension ref="A1:AS33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -767,34 +782,34 @@
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2">
-        <v>35077</v>
+        <v>37212</v>
       </c>
       <c r="E2" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G2" s="2">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -837,28 +852,28 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2">
-        <v>35077</v>
+        <v>37212</v>
       </c>
       <c r="E4" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G4" s="2">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4" s="2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -869,28 +884,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2">
-        <v>29764</v>
+        <v>30543</v>
       </c>
       <c r="E5" s="2">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I5" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -901,28 +916,28 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2">
-        <v>35722</v>
+        <v>37894</v>
       </c>
       <c r="E6" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="2">
+        <v>24</v>
+      </c>
+      <c r="H6" s="2">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="2">
-        <v>29</v>
-      </c>
-      <c r="H6" s="2">
-        <v>8</v>
-      </c>
       <c r="I6" s="2">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -933,15 +948,17 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2">
-        <v>23950</v>
+        <v>25032</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="2">
         <v>21</v>
       </c>
@@ -949,10 +966,10 @@
         <v>3</v>
       </c>
       <c r="I7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -963,28 +980,28 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2">
-        <v>33619</v>
+        <v>34951</v>
       </c>
       <c r="E8" s="2">
         <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G8" s="2">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -995,28 +1012,28 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2">
-        <v>35243</v>
+        <v>37251</v>
       </c>
       <c r="E9" s="2">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I9" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -1027,28 +1044,28 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2">
-        <v>36451</v>
+        <v>36795</v>
       </c>
       <c r="E10" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G10" s="2">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H10" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I10" s="2">
         <v>4</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -1059,16 +1076,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2">
-        <v>38267</v>
+        <v>40070</v>
       </c>
       <c r="E11" s="2">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1077,10 +1094,10 @@
         <v>32</v>
       </c>
       <c r="I11" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -1091,28 +1108,28 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2">
-        <v>28224</v>
+        <v>30079</v>
       </c>
       <c r="E12" s="2">
         <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G12" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H12" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I12" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -1123,28 +1140,28 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2">
-        <v>12401</v>
+        <v>12714</v>
       </c>
       <c r="E13" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G13" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13" s="2">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2">
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -1155,28 +1172,28 @@
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2">
-        <v>33949</v>
+        <v>35688</v>
       </c>
       <c r="E14" s="2">
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G14" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I14" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -1184,31 +1201,31 @@
         <v>21</v>
       </c>
       <c r="B15" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2">
-        <v>31250</v>
+        <v>30070</v>
       </c>
       <c r="E15" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G15" s="2">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="I15" s="2">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -1219,28 +1236,28 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2">
-        <v>34615</v>
+        <v>33410</v>
       </c>
       <c r="E16" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I16" s="2">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1251,28 +1268,28 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2">
-        <v>33572</v>
+        <v>30291</v>
       </c>
       <c r="E17" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G17" s="2">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="H17" s="2">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="I17" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1280,31 +1297,31 @@
         <v>24</v>
       </c>
       <c r="B18" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2">
-        <v>16174</v>
+        <v>33767</v>
       </c>
       <c r="E18" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G18" s="2">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H18" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1315,28 +1332,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="2">
-        <v>32002</v>
+        <v>32051</v>
       </c>
       <c r="E19" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G19" s="2">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H19" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I19" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1347,28 +1364,28 @@
         <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2">
-        <v>33527</v>
+        <v>34855</v>
       </c>
       <c r="E20" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G20" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H20" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I20" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1376,31 +1393,31 @@
         <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D21" s="2">
-        <v>31355</v>
+        <v>35134</v>
       </c>
       <c r="E21" s="2">
         <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G21" s="2">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="H21" s="2">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="I21" s="2">
         <v>12</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1411,28 +1428,28 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2">
-        <v>34890</v>
+        <v>32136</v>
       </c>
       <c r="E22" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H22" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I22" s="2">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1443,28 +1460,28 @@
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2">
-        <v>31476</v>
+        <v>36353</v>
       </c>
       <c r="E23" s="2">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="2">
+        <v>20</v>
+      </c>
+      <c r="H23" s="2">
         <v>12</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="2">
-        <v>26</v>
-      </c>
-      <c r="H23" s="2">
-        <v>19</v>
-      </c>
       <c r="I23" s="2">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1472,31 +1489,31 @@
         <v>30</v>
       </c>
       <c r="B24" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2">
-        <v>19847</v>
+        <v>33025</v>
       </c>
       <c r="E24" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G24" s="2">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H24" s="2">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="I24" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1507,28 +1524,28 @@
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2">
-        <v>37857</v>
+        <v>20183</v>
       </c>
       <c r="E25" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="2">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="I25" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1539,28 +1556,28 @@
         <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D26" s="2">
-        <v>38084</v>
+        <v>39987</v>
       </c>
       <c r="E26" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G26" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H26" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I26" s="2">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1568,31 +1585,31 @@
         <v>33</v>
       </c>
       <c r="B27" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2">
-        <v>8241</v>
+        <v>40293</v>
       </c>
       <c r="E27" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="2">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H27" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I27" s="2">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1603,28 +1620,28 @@
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2">
-        <v>6862</v>
+        <v>32994</v>
       </c>
       <c r="E28" s="2">
         <v>7</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G28" s="2">
+        <v>35</v>
+      </c>
+      <c r="H28" s="2">
+        <v>14</v>
+      </c>
+      <c r="I28" s="2">
         <v>5</v>
       </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>6</v>
-      </c>
       <c r="J28" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1635,26 +1652,28 @@
         <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="2">
-        <v>24874</v>
+        <v>9099</v>
       </c>
       <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="G29" s="2">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="H29" s="2">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="I29" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1662,31 +1681,31 @@
         <v>36</v>
       </c>
       <c r="B30" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="2">
-        <v>5474</v>
+        <v>7652</v>
       </c>
       <c r="E30" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G30" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="2">
         <v>1</v>
       </c>
       <c r="I30" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1697,16 +1716,16 @@
         <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2">
-        <v>31651</v>
+        <v>5554</v>
       </c>
       <c r="E31" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
@@ -1715,10 +1734,10 @@
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1729,28 +1748,60 @@
         <v>10</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D32" s="2">
-        <v>31160</v>
+        <v>32569</v>
       </c>
       <c r="E32" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G32" s="2">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="H32" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I32" s="2">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="2">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="2">
+        <v>31761</v>
+      </c>
+      <c r="E33" s="2">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="2">
+        <v>36</v>
+      </c>
+      <c r="H33" s="2">
+        <v>17</v>
+      </c>
+      <c r="I33" s="2">
+        <v>11</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1809,7 @@
     <mergeCell ref="A1:AS1"/>
     <mergeCell ref="A2:AS2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:H32">
+  <conditionalFormatting sqref="A2:H33">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD($B2,2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
highest pl score for c6
</commit_message>
<xml_diff>
--- a/output/c6/c6aurac_brawler_levels_team.xlsx
+++ b/output/c6/c6aurac_brawler_levels_team.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
   <si>
     <t>player</t>
   </si>
@@ -94,18 +94,18 @@
     <t>LA | FLASH</t>
   </si>
   <si>
-    <t>Saurav</t>
-  </si>
-  <si>
     <t>Snoopy&gt;.&lt;|をゆひせぬ</t>
   </si>
   <si>
-    <t>Blaze</t>
+    <t>Terrific🎃🎃🎃</t>
   </si>
   <si>
     <t>DOOM</t>
   </si>
   <si>
+    <t>The Legend</t>
+  </si>
+  <si>
     <t>eric</t>
   </si>
   <si>
@@ -118,12 +118,12 @@
     <t>☬ℝ𝔸𝕋𝕋𝕃𝔼ℝ☬</t>
   </si>
   <si>
+    <t>DØPExNÄVED</t>
+  </si>
+  <si>
     <t>IX|LIT</t>
   </si>
   <si>
-    <t>Mini Breeze</t>
-  </si>
-  <si>
     <t>Mini|Benn🎯</t>
   </si>
   <si>
@@ -184,18 +184,18 @@
     <t>#2YCQJ00Y</t>
   </si>
   <si>
-    <t>#U2Q9L2QU</t>
-  </si>
-  <si>
     <t>#C9RCCU8J</t>
   </si>
   <si>
-    <t>#C0R8YQC</t>
+    <t>#LQL0U9VP2</t>
   </si>
   <si>
     <t>#CPJC0QUV</t>
   </si>
   <si>
+    <t>#9PRLUPQJL</t>
+  </si>
+  <si>
     <t>#80VR8V9</t>
   </si>
   <si>
@@ -208,12 +208,12 @@
     <t>#89GV9UG9Q</t>
   </si>
   <si>
+    <t>#8V9QLR22Y</t>
+  </si>
+  <si>
     <t>#8V09Y2Y8</t>
   </si>
   <si>
-    <t>#2CVYPV0YP</t>
-  </si>
-  <si>
     <t>#9RVV02QQ</t>
   </si>
   <si>
@@ -226,37 +226,28 @@
     <t>#GJCYYV0P</t>
   </si>
   <si>
+    <t>Gold III</t>
+  </si>
+  <si>
+    <t>Silver III</t>
+  </si>
+  <si>
+    <t>Diamond II</t>
+  </si>
+  <si>
     <t>Diamond I</t>
   </si>
   <si>
-    <t>Silver III</t>
-  </si>
-  <si>
-    <t>Mythic I</t>
-  </si>
-  <si>
     <t>Diamond III</t>
   </si>
   <si>
-    <t>Diamond II</t>
+    <t>Gold I</t>
   </si>
   <si>
     <t>Gold II</t>
   </si>
   <si>
-    <t>Gold I</t>
-  </si>
-  <si>
-    <t>Gold III</t>
-  </si>
-  <si>
-    <t>Mythic II</t>
-  </si>
-  <si>
-    <t>Legend I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEA, BELLE, BIBI, BO, BROCK, BUSTER, BUZZ, BYRON, CARL, CHESTER, COLT, CROW, ... </t>
+    <t xml:space="preserve">AMBER, BEA, BELLE, BIBI, BO, BROCK, BULL, BUSTER, BUZZ, BYRON, CARL, CHESTER, ... </t>
   </si>
   <si>
     <t xml:space="preserve">BARLEY, BO, CROW, DARRYL, EMZ, EVE, JESSIE, NANI, NITA, PENNY, POCO, SANDY, ... </t>
@@ -271,7 +262,7 @@
     <t xml:space="preserve">ASH, BELLE, BO, BONNIE, BROCK, BUSTER, BUZZ, CARL, COLETTE, CROW, DARRYL, EMZ, ... </t>
   </si>
   <si>
-    <t xml:space="preserve">ASH, BEA, BELLE, BROCK, BUSTER, CARL, CHESTER, COLETTE, CROW, FANG, MORTIS, SPIKE, ... </t>
+    <t xml:space="preserve">ASH, BEA, BELLE, BROCK, BUSTER, CARL, CHESTER, COLETTE, CROW, FANG, MORTIS, POCO, ... </t>
   </si>
   <si>
     <t>8-BIT, ASH, BIBI, TICK</t>
@@ -295,27 +286,27 @@
     <t xml:space="preserve">8-BIT, AMBER, ASH, BELLE, BO, BONNIE, BROCK, BYRON, CHESTER, COLETTE, CROW, EDGAR, ... </t>
   </si>
   <si>
-    <t xml:space="preserve">BO, BROCK, CARL, COLT, DARRYL, FRANK, GALE, GENE, LEON, NITA, PAM, POCO, ... </t>
+    <t xml:space="preserve">BO, BONNIE, BROCK, CARL, COLT, CROW, DARRYL, EMZ, FRANK, GALE, GENE, LEON, ... </t>
   </si>
   <si>
     <t xml:space="preserve">BEA, BELLE, BO, BONNIE, BROCK, BUSTER, BUZZ, CARL, CHESTER, COLETTE, CROW, DARRYL, ... </t>
   </si>
   <si>
-    <t>COLETTE, COLT, CROW, FANG, MAX, MORTIS, STU, SURGE, TARA</t>
-  </si>
-  <si>
-    <t>BEA, CARL, COLT, EMZ, GENE, JACKY, MAX, MORTIS, SURGE, TARA</t>
+    <t>BO, COLETTE, COLT, CROW, FANG, MAX, MORTIS, STU, SURGE, TARA</t>
   </si>
   <si>
     <t>8-BIT, BUSTER, CHESTER, DYNAMIKE, EDGAR, EMZ, GRAY, MEG, PENNY, POCO, STU</t>
   </si>
   <si>
-    <t xml:space="preserve">BELLE, BUSTER, BYRON, CHESTER, CROW, GRIFF, GUS, JANET, OTIS, PIPER, POCO, SQUEAK, ... </t>
+    <t>CARL, COLT, RICO</t>
   </si>
   <si>
     <t xml:space="preserve">ASH, BEA, BELLE, BO, BONNIE, BUSTER, CARL, CHESTER, CROW, EMZ, EVE, GENE, ... </t>
   </si>
   <si>
+    <t>BULL, MORTIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASH, BELLE, EVE, GENE, GRIFF, LOLA, LOU, NANI, POCO, SPIKE, SPROUT, SURGE, ... </t>
   </si>
   <si>
@@ -328,12 +319,12 @@
     <t xml:space="preserve">AMBER, ASH, BEA, BELLE, BIBI, BO, BROCK, BUZZ, CARL, CHESTER, COLETTE, CROW, ... </t>
   </si>
   <si>
+    <t>COLT</t>
+  </si>
+  <si>
     <t>BIBI, CHESTER, MORTIS, RICO, TARA</t>
   </si>
   <si>
-    <t>MORTIS, RICO</t>
-  </si>
-  <si>
     <t>BO, DARRYL, LOLA, PAM, PENNY, RICO, SPIKE</t>
   </si>
   <si>
@@ -343,13 +334,13 @@
     <t xml:space="preserve">8-BIT, AMBER, ASH, BARLEY, BEA, BELLE, BIBI, BO, BONNIE, BROCK, BULL, BUSTER, ... </t>
   </si>
   <si>
-    <t>ASH, BYRON, CARL, EMZ, EVE, GENE, GRIFF, SANDY, SPIKE, SURGE</t>
+    <t xml:space="preserve">ASH, BYRON, CARL, CROW, EMZ, EVE, GENE, GRIFF, PAM, SANDY, SPIKE, STU, ... </t>
   </si>
   <si>
     <t>C6 Brawler Levels</t>
   </si>
   <si>
-    <t>2022-12-29</t>
+    <t>2023-01-04</t>
   </si>
 </sst>
 </file>
@@ -733,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -782,7 +773,7 @@
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -791,25 +782,25 @@
         <v>40</v>
       </c>
       <c r="D2" s="2">
-        <v>37212</v>
+        <v>37307</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2">
         <v>4</v>
       </c>
       <c r="I2" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -855,25 +846,25 @@
         <v>40</v>
       </c>
       <c r="D4" s="2">
-        <v>37212</v>
+        <v>37307</v>
       </c>
       <c r="E4" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G4" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2">
         <v>4</v>
       </c>
       <c r="I4" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -887,7 +878,7 @@
         <v>41</v>
       </c>
       <c r="D5" s="2">
-        <v>30543</v>
+        <v>30459</v>
       </c>
       <c r="E5" s="2">
         <v>6</v>
@@ -905,7 +896,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -919,25 +910,25 @@
         <v>42</v>
       </c>
       <c r="D6" s="2">
-        <v>37894</v>
+        <v>37930</v>
       </c>
       <c r="E6" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G6" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="2">
         <v>6</v>
       </c>
       <c r="I6" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -951,25 +942,25 @@
         <v>43</v>
       </c>
       <c r="D7" s="2">
-        <v>25032</v>
+        <v>24915</v>
       </c>
       <c r="E7" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G7" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" s="2">
         <v>8</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -983,14 +974,12 @@
         <v>44</v>
       </c>
       <c r="D8" s="2">
-        <v>34951</v>
+        <v>34985</v>
       </c>
       <c r="E8" s="2">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>73</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2">
         <v>22</v>
       </c>
@@ -1001,7 +990,7 @@
         <v>28</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -1015,25 +1004,25 @@
         <v>45</v>
       </c>
       <c r="D9" s="2">
-        <v>37251</v>
+        <v>37122</v>
       </c>
       <c r="E9" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9" s="2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H9" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I9" s="2">
         <v>15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -1047,13 +1036,13 @@
         <v>46</v>
       </c>
       <c r="D10" s="2">
-        <v>36795</v>
+        <v>36510</v>
       </c>
       <c r="E10" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G10" s="2">
         <v>18</v>
@@ -1065,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -1079,13 +1068,13 @@
         <v>47</v>
       </c>
       <c r="D11" s="2">
-        <v>40070</v>
+        <v>39691</v>
       </c>
       <c r="E11" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1094,10 +1083,10 @@
         <v>32</v>
       </c>
       <c r="I11" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -1111,10 +1100,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="2">
-        <v>30079</v>
+        <v>29705</v>
       </c>
       <c r="E12" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>75</v>
@@ -1129,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -1143,13 +1132,13 @@
         <v>49</v>
       </c>
       <c r="D13" s="2">
-        <v>12714</v>
+        <v>12763</v>
       </c>
       <c r="E13" s="2">
         <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="2">
         <v>3</v>
@@ -1161,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -1175,13 +1164,13 @@
         <v>50</v>
       </c>
       <c r="D14" s="2">
-        <v>35688</v>
+        <v>35489</v>
       </c>
       <c r="E14" s="2">
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G14" s="2">
         <v>30</v>
@@ -1193,7 +1182,7 @@
         <v>18</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -1207,13 +1196,13 @@
         <v>51</v>
       </c>
       <c r="D15" s="2">
-        <v>30070</v>
+        <v>29611</v>
       </c>
       <c r="E15" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="2">
         <v>2</v>
@@ -1222,10 +1211,10 @@
         <v>27</v>
       </c>
       <c r="I15" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -1239,25 +1228,25 @@
         <v>52</v>
       </c>
       <c r="D16" s="2">
-        <v>33410</v>
+        <v>33365</v>
       </c>
       <c r="E16" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1271,25 +1260,25 @@
         <v>53</v>
       </c>
       <c r="D17" s="2">
-        <v>30291</v>
+        <v>30422</v>
       </c>
       <c r="E17" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G17" s="2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H17" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I17" s="2">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1303,10 +1292,10 @@
         <v>54</v>
       </c>
       <c r="D18" s="2">
-        <v>33767</v>
+        <v>33469</v>
       </c>
       <c r="E18" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>72</v>
@@ -1318,10 +1307,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1335,10 +1324,10 @@
         <v>55</v>
       </c>
       <c r="D19" s="2">
-        <v>32051</v>
+        <v>31965</v>
       </c>
       <c r="E19" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>72</v>
@@ -1347,13 +1336,13 @@
         <v>37</v>
       </c>
       <c r="H19" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1367,25 +1356,25 @@
         <v>56</v>
       </c>
       <c r="D20" s="2">
-        <v>34855</v>
+        <v>34939</v>
       </c>
       <c r="E20" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G20" s="2">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="H20" s="2">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="I20" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1399,25 +1388,25 @@
         <v>57</v>
       </c>
       <c r="D21" s="2">
-        <v>35134</v>
+        <v>5240</v>
       </c>
       <c r="E21" s="2">
         <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G21" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="I21" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1431,25 +1420,25 @@
         <v>58</v>
       </c>
       <c r="D22" s="2">
-        <v>32136</v>
+        <v>36128</v>
       </c>
       <c r="E22" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G22" s="2">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H22" s="2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I22" s="2">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1463,25 +1452,23 @@
         <v>59</v>
       </c>
       <c r="D23" s="2">
-        <v>36353</v>
+        <v>5244</v>
       </c>
       <c r="E23" s="2">
-        <v>11</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I23" s="2">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1495,10 +1482,10 @@
         <v>60</v>
       </c>
       <c r="D24" s="2">
-        <v>33025</v>
+        <v>32684</v>
       </c>
       <c r="E24" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>72</v>
@@ -1510,10 +1497,10 @@
         <v>18</v>
       </c>
       <c r="I24" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1527,25 +1514,23 @@
         <v>61</v>
       </c>
       <c r="D25" s="2">
-        <v>20183</v>
+        <v>20349</v>
       </c>
       <c r="E25" s="2">
-        <v>16</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2">
         <v>2</v>
       </c>
       <c r="H25" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I25" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1559,14 +1544,12 @@
         <v>62</v>
       </c>
       <c r="D26" s="2">
-        <v>39987</v>
+        <v>39935</v>
       </c>
       <c r="E26" s="2">
-        <v>8</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F26" s="2"/>
       <c r="G26" s="2">
         <v>0</v>
       </c>
@@ -1577,7 +1560,7 @@
         <v>23</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1591,25 +1574,23 @@
         <v>63</v>
       </c>
       <c r="D27" s="2">
-        <v>40293</v>
+        <v>40012</v>
       </c>
       <c r="E27" s="2">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F27" s="2"/>
       <c r="G27" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I27" s="2">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1623,25 +1604,25 @@
         <v>64</v>
       </c>
       <c r="D28" s="2">
-        <v>32994</v>
+        <v>30178</v>
       </c>
       <c r="E28" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G28" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H28" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I28" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1655,25 +1636,25 @@
         <v>65</v>
       </c>
       <c r="D29" s="2">
-        <v>9099</v>
+        <v>32608</v>
       </c>
       <c r="E29" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G29" s="2">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H29" s="2">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I29" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1687,13 +1668,13 @@
         <v>66</v>
       </c>
       <c r="D30" s="2">
-        <v>7652</v>
+        <v>7758</v>
       </c>
       <c r="E30" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G30" s="2">
         <v>5</v>
@@ -1705,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1719,14 +1700,12 @@
         <v>67</v>
       </c>
       <c r="D31" s="2">
-        <v>5554</v>
+        <v>5458</v>
       </c>
       <c r="E31" s="2">
-        <v>16</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F31" s="2"/>
       <c r="G31" s="2">
         <v>0</v>
       </c>
@@ -1737,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1751,14 +1730,12 @@
         <v>68</v>
       </c>
       <c r="D32" s="2">
-        <v>32569</v>
+        <v>31989</v>
       </c>
       <c r="E32" s="2">
-        <v>13</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F32" s="2"/>
       <c r="G32" s="2">
         <v>0</v>
       </c>
@@ -1766,10 +1743,10 @@
         <v>0</v>
       </c>
       <c r="I32" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1783,25 +1760,25 @@
         <v>69</v>
       </c>
       <c r="D33" s="2">
-        <v>31761</v>
+        <v>31223</v>
       </c>
       <c r="E33" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G33" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H33" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I33" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix power levels bug
</commit_message>
<xml_diff>
--- a/output/c6/c6aurac_brawler_levels_team.xlsx
+++ b/output/c6/c6aurac_brawler_levels_team.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
   <si>
     <t>player</t>
   </si>
@@ -91,18 +91,12 @@
     <t>FuSiOn | ライオン🖤</t>
   </si>
   <si>
-    <t>LA | FLASH</t>
-  </si>
-  <si>
     <t>Silent killer</t>
   </si>
   <si>
     <t>DOOM</t>
   </si>
   <si>
-    <t>NRG |SARDORBEK</t>
-  </si>
-  <si>
     <t>eric</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>Terrific🎃🎃🎃</t>
   </si>
   <si>
-    <t>⚔Sword Emperor⚔</t>
-  </si>
-  <si>
     <t>LHC🥰DreamThree</t>
   </si>
   <si>
@@ -133,6 +124,15 @@
     <t>jem</t>
   </si>
   <si>
+    <t>Vierkay</t>
+  </si>
+  <si>
+    <t>Ys</t>
+  </si>
+  <si>
+    <t>जय श्री राम</t>
+  </si>
+  <si>
     <t>#JVQP8LLY</t>
   </si>
   <si>
@@ -178,18 +178,12 @@
     <t>#22Q2J2J</t>
   </si>
   <si>
-    <t>#2YCQJ00Y</t>
-  </si>
-  <si>
     <t>#LCUGVC9R0</t>
   </si>
   <si>
     <t>#CPJC0QUV</t>
   </si>
   <si>
-    <t>#9CV9RVCQL</t>
-  </si>
-  <si>
     <t>#80VR8V9</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
     <t>#LQL0U9VP2</t>
   </si>
   <si>
-    <t>#RV2RQQQC</t>
-  </si>
-  <si>
     <t>#LQQQ9YLL9</t>
   </si>
   <si>
@@ -220,6 +211,33 @@
     <t>#22LYUC8G8</t>
   </si>
   <si>
+    <t>#L2UVL80YC</t>
+  </si>
+  <si>
+    <t>#C00LQCUP</t>
+  </si>
+  <si>
+    <t>#CQYY0Y0</t>
+  </si>
+  <si>
+    <t>Diamond II</t>
+  </si>
+  <si>
+    <t>Gold II</t>
+  </si>
+  <si>
+    <t>Silver III</t>
+  </si>
+  <si>
+    <t>Diamond I</t>
+  </si>
+  <si>
+    <t>Diamond III</t>
+  </si>
+  <si>
+    <t>Bronze III</t>
+  </si>
+  <si>
     <t xml:space="preserve">AMBER, BEA, BELLE, BIBI, BO, BROCK, BULL, BUSTER, BUZZ, BYRON, CARL, CHESTER, ... </t>
   </si>
   <si>
@@ -256,22 +274,16 @@
     <t xml:space="preserve">8-BIT, AMBER, ASH, BELLE, BIBI, BO, BONNIE, BROCK, BUSTER, BUZZ, BYRON, CARL, ... </t>
   </si>
   <si>
-    <t xml:space="preserve">BO, BONNIE, BROCK, CARL, CHESTER, COLT, CROW, DARRYL, EMZ, FRANK, GALE, GENE, ... </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BO, COLETTE, COLT, CROW, EMZ, FANG, GENE, LEON, MAX, MORTIS, STU, SURGE, ... </t>
-  </si>
-  <si>
-    <t>8-BIT, ASH, BULL, FANG, GRIFF, GUS, LEON, SPIKE</t>
+    <t xml:space="preserve">BARLEY, BO, BONNIE, BROCK, CARL, CHESTER, COLT, CROW, DARRYL, EMZ, FRANK, GALE, ... </t>
+  </si>
+  <si>
+    <t>8-BIT, ASH, BULL, COLETTE, FANG, GRIFF, GUS, LEON, SPIKE</t>
   </si>
   <si>
     <t xml:space="preserve">ASH, BEA, BELLE, BO, BONNIE, BROCK, BUSTER, CARL, CHESTER, CROW, EMZ, EVE, ... </t>
   </si>
   <si>
-    <t>ASH, BO, BROCK, CROW, EVE, FANG, GALE, PENNY, SQUEAK, SURGE, TARA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASH, BELLE, EVE, GENE, GRIFF, GUS, LOLA, LOU, MEG, NANI, POCO, SPIKE, ... </t>
+    <t xml:space="preserve">ASH, BELLE, CARL, DYNAMIKE, EVE, GENE, GRIFF, GUS, LOLA, LOU, MAX, MEG, ... </t>
   </si>
   <si>
     <t xml:space="preserve">8-BIT, BARLEY, BONNIE, BROCK, CARL, CROW, DARRYL, EDGAR, EL PRIMO, EMZ, EVE, FANG, ... </t>
@@ -283,28 +295,34 @@
     <t xml:space="preserve">AMBER, ASH, BEA, BELLE, BIBI, BO, BROCK, BUSTER, BUZZ, CARL, CHESTER, COLETTE, ... </t>
   </si>
   <si>
-    <t>BO, CARL, NITA, PENNY</t>
+    <t>BO, CARL, COLETTE, NITA, PENNY</t>
   </si>
   <si>
     <t>BEA, CARL, COLT, JANET, POCO, RICO</t>
   </si>
   <si>
-    <t>CARL, CROW, EDGAR, MEG, MORTIS, PENNY, SPIKE, STU, SURGE, TARA</t>
-  </si>
-  <si>
     <t>CARL, DARRYL, FANG, GENE, GUS, JACKY, PENNY, RICO, TICK</t>
   </si>
   <si>
     <t>BROCK, CARL, PENNY</t>
   </si>
   <si>
-    <t>BROCK, GRIFF, SPIKE</t>
+    <t>BROCK, BUZZ, GRIFF, PENNY, SPIKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASH, BIBI, BO, BONNIE, BULL, CHESTER, COLT, CROW, DARRYL, EDGAR, EL PRIMO, EMZ, ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARLEY, BEA, BO, CROW, DARRYL, EMZ, EVE, JESSIE, NANI, NITA, PENNY, POCO, ... </t>
+  </si>
+  <si>
+    <t>COLT, CROW, EMZ, LEON, MAX, STU, TARA</t>
   </si>
   <si>
     <t>C6 Brawler Levels</t>
   </si>
   <si>
-    <t>2023-03-03</t>
+    <t>2023-03-07</t>
   </si>
 </sst>
 </file>
@@ -688,7 +706,7 @@
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -737,7 +755,7 @@
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -746,7 +764,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="2">
-        <v>37473</v>
+        <v>36382</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -762,7 +780,7 @@
         <v>45</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -808,7 +826,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="2">
-        <v>37473</v>
+        <v>36382</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -824,7 +842,7 @@
         <v>45</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -838,12 +856,14 @@
         <v>40</v>
       </c>
       <c r="D5" s="2">
-        <v>38760</v>
+        <v>38575</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G5" s="2">
         <v>16</v>
       </c>
@@ -854,7 +874,7 @@
         <v>45</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -868,12 +888,14 @@
         <v>41</v>
       </c>
       <c r="D6" s="2">
-        <v>25191</v>
+        <v>25444</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G6" s="2">
         <v>21</v>
       </c>
@@ -884,7 +906,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -898,7 +920,7 @@
         <v>42</v>
       </c>
       <c r="D7" s="2">
-        <v>36139</v>
+        <v>36060</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -914,7 +936,7 @@
         <v>30</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -928,12 +950,14 @@
         <v>43</v>
       </c>
       <c r="D8" s="2">
-        <v>39324</v>
+        <v>39014</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G8" s="2">
         <v>23</v>
       </c>
@@ -944,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -958,12 +982,14 @@
         <v>44</v>
       </c>
       <c r="D9" s="2">
-        <v>35673</v>
+        <v>34980</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G9" s="2">
         <v>16</v>
       </c>
@@ -974,7 +1000,7 @@
         <v>36</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -988,7 +1014,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="2">
-        <v>38513</v>
+        <v>37548</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -1004,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -1018,12 +1044,14 @@
         <v>46</v>
       </c>
       <c r="D11" s="2">
-        <v>42361</v>
+        <v>42103</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G11" s="2">
         <v>4</v>
       </c>
@@ -1034,7 +1062,7 @@
         <v>55</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -1048,23 +1076,25 @@
         <v>47</v>
       </c>
       <c r="D12" s="2">
-        <v>12997</v>
+        <v>13130</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="G12" s="2">
         <v>2</v>
       </c>
       <c r="H12" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I12" s="2">
         <v>4</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -1078,12 +1108,14 @@
         <v>48</v>
       </c>
       <c r="D13" s="2">
-        <v>37319</v>
+        <v>36632</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G13" s="2">
         <v>28</v>
       </c>
@@ -1094,7 +1126,7 @@
         <v>23</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -1108,12 +1140,14 @@
         <v>49</v>
       </c>
       <c r="D14" s="2">
-        <v>29923</v>
+        <v>29654</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
@@ -1124,7 +1158,7 @@
         <v>37</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -1138,12 +1172,14 @@
         <v>50</v>
       </c>
       <c r="D15" s="2">
-        <v>34479</v>
+        <v>34133</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G15" s="2">
         <v>8</v>
       </c>
@@ -1154,7 +1190,7 @@
         <v>49</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -1168,23 +1204,25 @@
         <v>51</v>
       </c>
       <c r="D16" s="2">
-        <v>33244</v>
+        <v>33203</v>
       </c>
       <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G16" s="2">
         <v>21</v>
       </c>
       <c r="H16" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I16" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1198,12 +1236,14 @@
         <v>52</v>
       </c>
       <c r="D17" s="2">
-        <v>34894</v>
+        <v>34634</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G17" s="2">
         <v>14</v>
       </c>
@@ -1214,7 +1254,7 @@
         <v>50</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1228,17 +1268,19 @@
         <v>53</v>
       </c>
       <c r="D18" s="2">
-        <v>40505</v>
+        <v>39822</v>
       </c>
       <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G18" s="2">
         <v>44</v>
       </c>
       <c r="H18" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1256,23 +1298,25 @@
         <v>54</v>
       </c>
       <c r="D19" s="2">
-        <v>35356</v>
+        <v>32511</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="G19" s="2">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="H19" s="2">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="I19" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1280,29 +1324,31 @@
         <v>26</v>
       </c>
       <c r="B20" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D20" s="2">
-        <v>32702</v>
+        <v>36605</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G20" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" s="2">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="I20" s="2">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1316,23 +1362,25 @@
         <v>56</v>
       </c>
       <c r="D21" s="2">
-        <v>37280</v>
+        <v>35129</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G21" s="2">
         <v>21</v>
       </c>
       <c r="H21" s="2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I21" s="2">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1340,29 +1388,29 @@
         <v>28</v>
       </c>
       <c r="B22" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D22" s="2">
-        <v>29475</v>
+        <v>21139</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H22" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I22" s="2">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1370,29 +1418,31 @@
         <v>29</v>
       </c>
       <c r="B23" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D23" s="2">
-        <v>35439</v>
+        <v>40759</v>
       </c>
       <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G23" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="I23" s="2">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1406,23 +1456,23 @@
         <v>59</v>
       </c>
       <c r="D24" s="2">
-        <v>21211</v>
+        <v>38681</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H24" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I24" s="2">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1430,29 +1480,31 @@
         <v>31</v>
       </c>
       <c r="B25" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="2">
-        <v>40959</v>
+        <v>7114</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
       <c r="H25" s="2">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="I25" s="2">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1460,29 +1512,29 @@
         <v>32</v>
       </c>
       <c r="B26" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="2">
-        <v>39958</v>
+        <v>6463</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I26" s="2">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1490,29 +1542,29 @@
         <v>33</v>
       </c>
       <c r="B27" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="2">
-        <v>6050</v>
+        <v>6283</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1520,29 +1572,31 @@
         <v>34</v>
       </c>
       <c r="B28" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="2">
-        <v>6050</v>
+        <v>6376</v>
       </c>
       <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1550,119 +1604,117 @@
         <v>35</v>
       </c>
       <c r="B29" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="2">
-        <v>35601</v>
+        <v>36038</v>
       </c>
       <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G29" s="2">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H29" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I29" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="2">
-        <v>10</v>
-      </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="2">
-        <v>6316</v>
+        <v>35001</v>
       </c>
       <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H30" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I30" s="2">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="2">
-        <v>10</v>
-      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="2">
-        <v>6180</v>
+        <v>30870</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="H31" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I31" s="2">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="2">
-        <v>10</v>
-      </c>
+      <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="2">
-        <v>36200</v>
+        <v>29785</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H32" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I32" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1722,7 @@
     <mergeCell ref="A1:AS1"/>
     <mergeCell ref="A2:AS2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:H32">
+  <conditionalFormatting sqref="A2:H29">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD($B2,2)=0</formula>
     </cfRule>

</xml_diff>